<commit_message>
MR adding another IP
</commit_message>
<xml_diff>
--- a/manual/mr/mr_Investigation_results.xlsx
+++ b/manual/mr/mr_Investigation_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reiterm/Programing/AAU/let-me-out/manual/mr/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AAU\let-me-out\manual\mr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC8E146-DEB7-F042-9FBC-16CCDCCB7231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF82DE94-B3EB-43F7-A668-B157E953E4B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10940" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munkalap1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="75">
   <si>
     <t>IP address</t>
   </si>
@@ -142,12 +142,6 @@
     <t>Slagelse</t>
   </si>
   <si>
-    <t>ASN</t>
-  </si>
-  <si>
-    <t>abuseipdb: 1%</t>
-  </si>
-  <si>
     <t>Web Spam</t>
   </si>
   <si>
@@ -163,9 +157,6 @@
     <t>IP camera</t>
   </si>
   <si>
-    <t>virustotal, abuseipdb, shodan, mxtoolbox, whois lookup, bgpview.io</t>
-  </si>
-  <si>
     <t>Probably trojan spamming and/or TOR endpoint</t>
   </si>
   <si>
@@ -212,6 +203,48 @@
   </si>
   <si>
     <t>autodiscover.gsl.dk, autodiscover.lynge.org, lynge.vip, cups.lynge.org, smtpauth.ancher.net, gw.lynge.org, thor.gsl.dk, mx10.lynge.org, sniper.gsl.dk, mails.lynge.org</t>
+  </si>
+  <si>
+    <t>85.218.200.182</t>
+  </si>
+  <si>
+    <t>85.218.128.0/17</t>
+  </si>
+  <si>
+    <t>Norlys Digital A/S</t>
+  </si>
+  <si>
+    <t>Vemmelev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abusix Mail Intelligence Blacklist, BLOCKLIST.DE, INTERSERVER, s5h.net, SPAMCOP, Spamhaus ZEN, UCEPROTECTL1, UCEPROTECTL2 </t>
+  </si>
+  <si>
+    <t>virustotal: 6+3, abuseipdb: 100%</t>
+  </si>
+  <si>
+    <t>virustotal: 2, abuseipdb: 1%</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>Brute-Force, Web App Attack, Hacking, DDoS, E-mail Spam, Exploited Host</t>
+  </si>
+  <si>
+    <t>19 FTP (?), 22 SSH, 80 HTTP, 111 ONC-RPC (Portmapper), 137 NetBIOS, 443 HTTPS, 445 SMB, 1900 SSDP, 3265/UNKNOWN, 5000 UPNP, 5001 HTTPS, 5357 HTTP, 9091 HTTP</t>
+  </si>
+  <si>
+    <t>HTTP Response 502, 403, 302</t>
+  </si>
+  <si>
+    <t>Maybe home router</t>
+  </si>
+  <si>
+    <t>virustotal, abuseipdb, shodan, mxtoolbox, whois lookup, bgpview.io, censys, viewdns</t>
+  </si>
+  <si>
+    <t>Many ports open, many services, looks like a home router or server, FTP, NAS, SSH, multiple HTTP, very weird, and lot of attacks</t>
   </si>
 </sst>
 </file>
@@ -311,23 +344,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -543,72 +579,73 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" customWidth="1"/>
-    <col min="3" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.6640625" customWidth="1"/>
-    <col min="9" max="9" width="37.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="49.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="59.1640625" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" customWidth="1"/>
-    <col min="13" max="13" width="18.33203125" customWidth="1"/>
-    <col min="14" max="14" width="20.5" customWidth="1"/>
-    <col min="15" max="15" width="16.6640625" customWidth="1"/>
-    <col min="16" max="16" width="49" customWidth="1"/>
-    <col min="17" max="17" width="38.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="54.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="123.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="110.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="219.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="141.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" customWidth="1"/>
+    <col min="16" max="16" width="55" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="111.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="73" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
+    <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
     </row>
-    <row r="3" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,7 +701,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -720,116 +757,172 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:18" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="7" t="s">
+      <c r="J5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" s="6">
+        <v>45224</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q5" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="L5" s="7" t="s">
+      <c r="R5" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="M5" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="N5" s="7" t="s">
+      <c r="E6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="O5" s="8">
-        <v>45224</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>47</v>
+      <c r="H6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" t="s">
+        <v>59</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O6" s="7">
+        <v>43691</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" s="7" t="s">
+    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I6" s="7" t="s">
+      <c r="F7" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="K7" t="s">
+        <v>46</v>
+      </c>
+      <c r="L7" t="s">
+        <v>71</v>
+      </c>
+      <c r="M7" t="s">
+        <v>46</v>
+      </c>
+      <c r="N7" t="s">
+        <v>72</v>
+      </c>
+      <c r="O7" s="7">
+        <v>45232</v>
+      </c>
+      <c r="P7" t="s">
         <v>55</v>
       </c>
-      <c r="J6" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="K6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="M6" t="s">
-        <v>63</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="O6" s="10">
-        <v>43691</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q6" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="R6" s="9" t="s">
-        <v>47</v>
+      <c r="Q7" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>